<commit_message>
Tích hợp Google Analytics và thêm thông báo
</commit_message>
<xml_diff>
--- a/DSKH.xlsx
+++ b/DSKH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HNT24\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6D0050-421A-4F87-8D85-B0CDDBCE5F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5D5AA5-EBE6-4BC3-A722-13DD9EE5F9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="683">
   <si>
     <t>STT</t>
   </si>
@@ -2078,6 +2078,15 @@
   </si>
   <si>
     <t>0100109106-011</t>
+  </si>
+  <si>
+    <t>CÔNG TY CỔ PHẦN MP LOGISTICS</t>
+  </si>
+  <si>
+    <t>0315266412</t>
+  </si>
+  <si>
+    <t>KHTV.143</t>
   </si>
 </sst>
 </file>
@@ -2239,17 +2248,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{72968E78-4D5E-40B5-8606-A1CA43B72489}"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2509,10 +2508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E243"/>
+  <dimension ref="A1:E244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="B245" sqref="B245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -5485,7 +5484,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="14">
-        <f t="shared" ref="A196:A243" si="3">+A195+1</f>
+        <f t="shared" ref="A196:A244" si="3">+A195+1</f>
         <v>195</v>
       </c>
       <c r="B196" s="20" t="s">
@@ -6203,9 +6202,24 @@
         <v>669</v>
       </c>
     </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" s="14">
+        <f t="shared" si="3"/>
+        <v>243</v>
+      </c>
+      <c r="B244" s="20" t="s">
+        <v>680</v>
+      </c>
+      <c r="C244" s="21" t="s">
+        <v>681</v>
+      </c>
+      <c r="D244" s="19" t="s">
+        <v>682</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Cập nhật khách hàng
</commit_message>
<xml_diff>
--- a/DSKH.xlsx
+++ b/DSKH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5D5AA5-EBE6-4BC3-A722-13DD9EE5F9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6A6370-7761-40E7-8208-E86A1B202D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="680">
   <si>
     <t>STT</t>
   </si>
@@ -1612,9 +1612,6 @@
     <t>Công ty Cổ phần Đầu tư Thương mại và Du lịch Anh Thư</t>
   </si>
   <si>
-    <t>Doanh nghiệp tư nhân Trúc Mai NB</t>
-  </si>
-  <si>
     <t>Công ty Cổ phần Gạch Cầu Rào</t>
   </si>
   <si>
@@ -1786,9 +1783,6 @@
     <t>KHTV.127</t>
   </si>
   <si>
-    <t>KHTV133</t>
-  </si>
-  <si>
     <t>KHTV99</t>
   </si>
   <si>
@@ -1922,9 +1916,6 @@
   </si>
   <si>
     <t>KHTV09</t>
-  </si>
-  <si>
-    <t>KHTV03</t>
   </si>
   <si>
     <t>KHTV.123</t>
@@ -2248,7 +2239,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{72968E78-4D5E-40B5-8606-A1CA43B72489}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2508,22 +2519,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E244"/>
+  <dimension ref="A1:E242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
-      <selection activeCell="B245" sqref="B245"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2538,7 +2549,7 @@
       </c>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -2553,7 +2564,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <f>+A2+1</f>
         <v>2</v>
@@ -2569,7 +2580,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="14">
         <f t="shared" ref="A4:A67" si="0">+A3+1</f>
         <v>3</v>
@@ -2585,7 +2596,7 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2601,7 +2612,7 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2617,7 +2628,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2633,7 +2644,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2649,7 +2660,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="14">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2665,7 +2676,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2681,7 +2692,7 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="14">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2697,7 +2708,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2713,7 +2724,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2729,7 +2740,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2745,7 +2756,7 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2761,7 +2772,7 @@
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2777,7 +2788,7 @@
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="14">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2793,7 +2804,7 @@
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2809,7 +2820,7 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2825,7 +2836,7 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2841,7 +2852,7 @@
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2857,7 +2868,7 @@
       </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2873,7 +2884,7 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2889,7 +2900,7 @@
       </c>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2905,7 +2916,7 @@
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="14">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2921,7 +2932,7 @@
       </c>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2937,7 +2948,7 @@
       </c>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="14">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2953,7 +2964,7 @@
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="14">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2969,7 +2980,7 @@
       </c>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="14">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2985,7 +2996,7 @@
       </c>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="14">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3001,7 +3012,7 @@
       </c>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3017,7 +3028,7 @@
       </c>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="14">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3033,7 +3044,7 @@
       </c>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="14">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3049,7 +3060,7 @@
       </c>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="14">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3065,7 +3076,7 @@
       </c>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="14">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3081,7 +3092,7 @@
       </c>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="14">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3097,7 +3108,7 @@
       </c>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="14">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3113,7 +3124,7 @@
       </c>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="14">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3129,7 +3140,7 @@
       </c>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="14">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3145,7 +3156,7 @@
       </c>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3161,7 +3172,7 @@
       </c>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="14">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3177,7 +3188,7 @@
       </c>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="14">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3193,7 +3204,7 @@
       </c>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3209,7 +3220,7 @@
       </c>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3225,7 +3236,7 @@
       </c>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="14">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3241,7 +3252,7 @@
       </c>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="14">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3257,7 +3268,7 @@
       </c>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="14">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3272,7 +3283,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="14">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3287,7 +3298,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="14">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -3302,7 +3313,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="14">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -3317,7 +3328,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -3332,7 +3343,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="14">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -3347,7 +3358,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="14">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -3362,7 +3373,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="14">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -3377,7 +3388,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="14">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -3392,7 +3403,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="14">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -3407,7 +3418,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="14">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -3422,7 +3433,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="14">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -3437,7 +3448,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="14">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -3452,7 +3463,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="14">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -3467,7 +3478,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="14">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -3482,7 +3493,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="14">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -3497,7 +3508,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="14">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -3512,7 +3523,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="14">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -3527,7 +3538,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="14">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -3542,7 +3553,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="14">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -3557,7 +3568,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="14">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -3572,7 +3583,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="14">
         <f t="shared" ref="A68:A131" si="1">+A67+1</f>
         <v>67</v>
@@ -3587,7 +3598,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="14">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -3602,7 +3613,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="14">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -3617,7 +3628,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="14">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -3632,7 +3643,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="14">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -3647,7 +3658,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="14">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -3662,7 +3673,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="14">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -3677,7 +3688,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="14">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -3692,7 +3703,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="14">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -3707,7 +3718,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="14">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -3722,7 +3733,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="14">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -3737,7 +3748,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="14">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -3752,7 +3763,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="14">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -3767,7 +3778,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="14">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -3782,7 +3793,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="14">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -3797,7 +3808,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="14">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -3812,7 +3823,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="14">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -3827,7 +3838,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="14">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -3842,7 +3853,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="14">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -3857,7 +3868,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="14">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -3872,7 +3883,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="14">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -3887,7 +3898,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="14">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -3902,7 +3913,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="14">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -3917,7 +3928,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="14">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -3932,7 +3943,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="14">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -3947,7 +3958,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="14">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -3962,7 +3973,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="14">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -3977,7 +3988,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="14">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -3992,7 +4003,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="14">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -4007,7 +4018,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="14">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -4022,7 +4033,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="14">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -4037,7 +4048,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="14">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -4052,7 +4063,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="14">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -4065,7 +4076,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="14">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4078,7 +4089,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="14">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -4091,7 +4102,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="14">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -4106,7 +4117,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="14">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -4121,7 +4132,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="14">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -4134,7 +4145,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="14">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -4147,7 +4158,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="14">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -4162,7 +4173,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="14">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -4177,7 +4188,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="14">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -4192,7 +4203,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="14">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -4207,7 +4218,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="14">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -4222,7 +4233,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="14">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -4237,7 +4248,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="14">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -4252,7 +4263,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="14">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -4267,7 +4278,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="14">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -4282,7 +4293,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="14">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -4297,7 +4308,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="14">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -4312,7 +4323,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="14">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -4327,7 +4338,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="14">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -4342,7 +4353,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="14">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -4357,7 +4368,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="14">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -4372,7 +4383,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="14">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -4387,7 +4398,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="14">
         <f t="shared" si="1"/>
         <v>122</v>
@@ -4402,7 +4413,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="14">
         <f t="shared" si="1"/>
         <v>123</v>
@@ -4417,7 +4428,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="14">
         <f t="shared" si="1"/>
         <v>124</v>
@@ -4432,7 +4443,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="14">
         <f t="shared" si="1"/>
         <v>125</v>
@@ -4447,7 +4458,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="14">
         <f t="shared" si="1"/>
         <v>126</v>
@@ -4462,7 +4473,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="14">
         <f t="shared" si="1"/>
         <v>127</v>
@@ -4477,7 +4488,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="14">
         <f t="shared" si="1"/>
         <v>128</v>
@@ -4492,7 +4503,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="14">
         <f t="shared" si="1"/>
         <v>129</v>
@@ -4507,7 +4518,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="14">
         <f t="shared" si="1"/>
         <v>130</v>
@@ -4522,7 +4533,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="14">
         <f t="shared" ref="A132:A195" si="2">+A131+1</f>
         <v>131</v>
@@ -4537,7 +4548,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="14">
         <f t="shared" si="2"/>
         <v>132</v>
@@ -4552,7 +4563,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="14">
         <f t="shared" si="2"/>
         <v>133</v>
@@ -4567,7 +4578,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="14">
         <f t="shared" si="2"/>
         <v>134</v>
@@ -4582,7 +4593,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="14">
         <f t="shared" si="2"/>
         <v>135</v>
@@ -4597,7 +4608,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="14">
         <f t="shared" si="2"/>
         <v>136</v>
@@ -4612,7 +4623,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="14">
         <f t="shared" si="2"/>
         <v>137</v>
@@ -4627,7 +4638,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="14">
         <f t="shared" si="2"/>
         <v>138</v>
@@ -4642,7 +4653,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="14">
         <f t="shared" si="2"/>
         <v>139</v>
@@ -4651,13 +4662,13 @@
         <v>463</v>
       </c>
       <c r="C140" s="21" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="D140" s="19" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="14">
         <f t="shared" si="2"/>
         <v>140</v>
@@ -4666,13 +4677,13 @@
         <v>464</v>
       </c>
       <c r="C141" s="21" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="D141" s="19" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="14">
         <f t="shared" si="2"/>
         <v>141</v>
@@ -4681,13 +4692,13 @@
         <v>465</v>
       </c>
       <c r="C142" s="21" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="D142" s="19" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="14">
         <f t="shared" si="2"/>
         <v>142</v>
@@ -4696,13 +4707,13 @@
         <v>466</v>
       </c>
       <c r="C143" s="21" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="D143" s="19" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="14">
         <f t="shared" si="2"/>
         <v>143</v>
@@ -4711,13 +4722,13 @@
         <v>467</v>
       </c>
       <c r="C144" s="21" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="D144" s="19" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="14">
         <f t="shared" si="2"/>
         <v>144</v>
@@ -4726,13 +4737,13 @@
         <v>468</v>
       </c>
       <c r="C145" s="21" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="D145" s="19" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="14">
         <f t="shared" si="2"/>
         <v>145</v>
@@ -4741,13 +4752,13 @@
         <v>469</v>
       </c>
       <c r="C146" s="21" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="D146" s="19" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="14">
         <f t="shared" si="2"/>
         <v>146</v>
@@ -4756,13 +4767,13 @@
         <v>470</v>
       </c>
       <c r="C147" s="21" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D147" s="19" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="14">
         <f t="shared" si="2"/>
         <v>147</v>
@@ -4771,13 +4782,13 @@
         <v>471</v>
       </c>
       <c r="C148" s="21" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="D148" s="19" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="14">
         <f t="shared" si="2"/>
         <v>148</v>
@@ -4786,13 +4797,13 @@
         <v>472</v>
       </c>
       <c r="C149" s="21" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="D149" s="19" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="14">
         <f t="shared" si="2"/>
         <v>149</v>
@@ -4800,14 +4811,12 @@
       <c r="B150" s="20" t="s">
         <v>473</v>
       </c>
-      <c r="C150" s="21" t="s">
-        <v>121</v>
-      </c>
+      <c r="C150" s="21"/>
       <c r="D150" s="19" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="14">
         <f t="shared" si="2"/>
         <v>150</v>
@@ -4819,10 +4828,10 @@
         <v>2700891595</v>
       </c>
       <c r="D151" s="19" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="14">
         <f t="shared" si="2"/>
         <v>151</v>
@@ -4834,10 +4843,10 @@
         <v>2700544577</v>
       </c>
       <c r="D152" s="19" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="14">
         <f t="shared" si="2"/>
         <v>152</v>
@@ -4849,10 +4858,10 @@
         <v>390</v>
       </c>
       <c r="D153" s="19" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="14">
         <f t="shared" si="2"/>
         <v>153</v>
@@ -4864,10 +4873,10 @@
         <v>391</v>
       </c>
       <c r="D154" s="19" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="14">
         <f t="shared" si="2"/>
         <v>154</v>
@@ -4879,1347 +4888,1320 @@
         <v>392</v>
       </c>
       <c r="D155" s="19" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="14">
         <f t="shared" si="2"/>
         <v>155</v>
       </c>
       <c r="B156" s="20" t="s">
-        <v>80</v>
+        <v>479</v>
       </c>
       <c r="C156" s="21" t="s">
-        <v>81</v>
+        <v>393</v>
       </c>
       <c r="D156" s="19" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="14">
         <f t="shared" si="2"/>
         <v>156</v>
       </c>
       <c r="B157" s="20" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C157" s="21" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D157" s="19" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="14">
         <f t="shared" si="2"/>
         <v>157</v>
       </c>
       <c r="B158" s="20" t="s">
-        <v>480</v>
-      </c>
-      <c r="C158" s="21" t="s">
-        <v>394</v>
+        <v>481</v>
+      </c>
+      <c r="C158" s="21">
+        <v>2802900665</v>
       </c>
       <c r="D158" s="19" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="14">
         <f t="shared" si="2"/>
         <v>158</v>
       </c>
       <c r="B159" s="20" t="s">
-        <v>481</v>
-      </c>
-      <c r="C159" s="21">
-        <v>2802900665</v>
+        <v>482</v>
+      </c>
+      <c r="C159" s="21" t="s">
+        <v>395</v>
       </c>
       <c r="D159" s="19" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="14">
         <f t="shared" si="2"/>
         <v>159</v>
       </c>
       <c r="B160" s="20" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C160" s="21" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D160" s="19" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="14">
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
       <c r="B161" s="20" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C161" s="21" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D161" s="19" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="14">
         <f t="shared" si="2"/>
         <v>161</v>
       </c>
       <c r="B162" s="20" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C162" s="21" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D162" s="19" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="14">
         <f t="shared" si="2"/>
         <v>162</v>
       </c>
       <c r="B163" s="20" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C163" s="21" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D163" s="19" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="14">
         <f t="shared" si="2"/>
         <v>163</v>
       </c>
       <c r="B164" s="20" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C164" s="21" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D164" s="19" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="14">
         <f t="shared" si="2"/>
         <v>164</v>
       </c>
       <c r="B165" s="20" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C165" s="21" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D165" s="19" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="14">
         <f t="shared" si="2"/>
         <v>165</v>
       </c>
       <c r="B166" s="20" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C166" s="21" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D166" s="19" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="14">
         <f t="shared" si="2"/>
         <v>166</v>
       </c>
       <c r="B167" s="20" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C167" s="21" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D167" s="19" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="14">
         <f t="shared" si="2"/>
         <v>167</v>
       </c>
       <c r="B168" s="20" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C168" s="21" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D168" s="19" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="14">
         <f t="shared" si="2"/>
         <v>168</v>
       </c>
       <c r="B169" s="20" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C169" s="21" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D169" s="19" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="14">
         <f t="shared" si="2"/>
         <v>169</v>
       </c>
       <c r="B170" s="20" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C170" s="21" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D170" s="19" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="14">
         <f t="shared" si="2"/>
         <v>170</v>
       </c>
       <c r="B171" s="20" t="s">
-        <v>493</v>
-      </c>
-      <c r="C171" s="21" t="s">
-        <v>406</v>
+        <v>494</v>
+      </c>
+      <c r="C171" s="21">
+        <v>3701760678</v>
       </c>
       <c r="D171" s="19" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="14">
         <f t="shared" si="2"/>
         <v>171</v>
       </c>
       <c r="B172" s="20" t="s">
-        <v>494</v>
-      </c>
-      <c r="C172" s="21">
-        <v>3701760678</v>
+        <v>495</v>
+      </c>
+      <c r="C172" s="21" t="s">
+        <v>407</v>
       </c>
       <c r="D172" s="19" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="14">
         <f t="shared" si="2"/>
         <v>172</v>
       </c>
       <c r="B173" s="20" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C173" s="21" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D173" s="19" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="14">
         <f t="shared" si="2"/>
         <v>173</v>
       </c>
       <c r="B174" s="20" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C174" s="21" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D174" s="19" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="14">
         <f t="shared" si="2"/>
         <v>174</v>
       </c>
       <c r="B175" s="20" t="s">
-        <v>497</v>
-      </c>
-      <c r="C175" s="21" t="s">
-        <v>409</v>
+        <v>498</v>
+      </c>
+      <c r="C175" s="21">
+        <v>6300227884</v>
       </c>
       <c r="D175" s="19" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="14">
         <f t="shared" si="2"/>
         <v>175</v>
       </c>
       <c r="B176" s="20" t="s">
-        <v>498</v>
-      </c>
-      <c r="C176" s="21">
-        <v>6300227884</v>
+        <v>499</v>
+      </c>
+      <c r="C176" s="21" t="s">
+        <v>410</v>
       </c>
       <c r="D176" s="19" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="14">
         <f t="shared" si="2"/>
         <v>176</v>
       </c>
       <c r="B177" s="20" t="s">
-        <v>499</v>
-      </c>
-      <c r="C177" s="21" t="s">
-        <v>410</v>
+        <v>500</v>
+      </c>
+      <c r="C177" s="21">
+        <v>3002131839</v>
       </c>
       <c r="D177" s="19" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="14">
         <f t="shared" si="2"/>
         <v>177</v>
       </c>
       <c r="B178" s="20" t="s">
-        <v>500</v>
-      </c>
-      <c r="C178" s="21">
-        <v>3002131839</v>
+        <v>501</v>
+      </c>
+      <c r="C178" s="21" t="s">
+        <v>411</v>
       </c>
       <c r="D178" s="19" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="14">
         <f t="shared" si="2"/>
         <v>178</v>
       </c>
       <c r="B179" s="20" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C179" s="21" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D179" s="19" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="14">
         <f t="shared" si="2"/>
         <v>179</v>
       </c>
       <c r="B180" s="20" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C180" s="21" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D180" s="19" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="14">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="B181" s="20" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C181" s="21" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D181" s="19" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="14">
         <f t="shared" si="2"/>
         <v>181</v>
       </c>
       <c r="B182" s="20" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C182" s="21" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D182" s="19" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="14">
         <f t="shared" si="2"/>
         <v>182</v>
       </c>
       <c r="B183" s="20" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C183" s="21" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D183" s="19" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="14">
         <f t="shared" si="2"/>
         <v>183</v>
       </c>
       <c r="B184" s="20" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C184" s="21" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D184" s="19" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="14">
         <f t="shared" si="2"/>
         <v>184</v>
       </c>
       <c r="B185" s="20" t="s">
-        <v>507</v>
-      </c>
-      <c r="C185" s="21" t="s">
-        <v>417</v>
+        <v>508</v>
+      </c>
+      <c r="C185" s="21">
+        <v>2902037650</v>
       </c>
       <c r="D185" s="19" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="14">
         <f t="shared" si="2"/>
         <v>185</v>
       </c>
       <c r="B186" s="20" t="s">
-        <v>508</v>
-      </c>
-      <c r="C186" s="21">
-        <v>2902037650</v>
+        <v>509</v>
+      </c>
+      <c r="C186" s="21" t="s">
+        <v>418</v>
       </c>
       <c r="D186" s="19" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="14">
         <f t="shared" si="2"/>
         <v>186</v>
       </c>
       <c r="B187" s="20" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C187" s="21" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D187" s="19" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="14">
         <f t="shared" si="2"/>
         <v>187</v>
       </c>
       <c r="B188" s="20" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C188" s="21" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D188" s="19" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="14">
         <f t="shared" si="2"/>
         <v>188</v>
       </c>
       <c r="B189" s="20" t="s">
-        <v>511</v>
-      </c>
-      <c r="C189" s="21" t="s">
-        <v>420</v>
+        <v>512</v>
+      </c>
+      <c r="C189" s="21">
+        <v>2901337179</v>
       </c>
       <c r="D189" s="19" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="14">
         <f t="shared" si="2"/>
         <v>189</v>
       </c>
       <c r="B190" s="20" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C190" s="21">
-        <v>2901337179</v>
+        <v>2901876974</v>
       </c>
       <c r="D190" s="19" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="14">
         <f t="shared" si="2"/>
         <v>190</v>
       </c>
       <c r="B191" s="20" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C191" s="21">
-        <v>2901876974</v>
+        <v>0</v>
       </c>
       <c r="D191" s="19" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="14">
         <f t="shared" si="2"/>
         <v>191</v>
       </c>
       <c r="B192" s="20" t="s">
-        <v>514</v>
-      </c>
-      <c r="C192" s="21">
-        <v>0</v>
+        <v>515</v>
+      </c>
+      <c r="C192" s="21" t="s">
+        <v>421</v>
       </c>
       <c r="D192" s="19" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="14">
         <f t="shared" si="2"/>
         <v>192</v>
       </c>
       <c r="B193" s="20" t="s">
-        <v>515</v>
-      </c>
-      <c r="C193" s="21" t="s">
-        <v>421</v>
+        <v>516</v>
+      </c>
+      <c r="C193" s="21">
+        <v>2802498400</v>
       </c>
       <c r="D193" s="19" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="14">
         <f t="shared" si="2"/>
         <v>193</v>
       </c>
       <c r="B194" s="20" t="s">
-        <v>516</v>
-      </c>
-      <c r="C194" s="21">
-        <v>2802498400</v>
+        <v>517</v>
+      </c>
+      <c r="C194" s="21" t="s">
+        <v>422</v>
       </c>
       <c r="D194" s="19" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="14">
         <f t="shared" si="2"/>
         <v>194</v>
       </c>
       <c r="B195" s="20" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C195" s="21" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D195" s="19" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A196" s="14">
+        <f t="shared" ref="A196:A242" si="3">+A195+1</f>
+        <v>195</v>
+      </c>
+      <c r="B196" s="20" t="s">
+        <v>519</v>
+      </c>
+      <c r="C196" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="D196" s="19" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="14">
-        <f t="shared" ref="A196:A244" si="3">+A195+1</f>
-        <v>195</v>
-      </c>
-      <c r="B196" s="20" t="s">
-        <v>518</v>
-      </c>
-      <c r="C196" s="21" t="s">
-        <v>423</v>
-      </c>
-      <c r="D196" s="19" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="14">
         <f t="shared" si="3"/>
         <v>196</v>
       </c>
       <c r="B197" s="20" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C197" s="21" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D197" s="19" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="14">
         <f t="shared" si="3"/>
         <v>197</v>
       </c>
       <c r="B198" s="20" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C198" s="21" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D198" s="19" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="14">
         <f t="shared" si="3"/>
         <v>198</v>
       </c>
       <c r="B199" s="20" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C199" s="21" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D199" s="19" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="14">
         <f t="shared" si="3"/>
         <v>199</v>
       </c>
       <c r="B200" s="20" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C200" s="21" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D200" s="19" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="14">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="B201" s="20" t="s">
-        <v>523</v>
-      </c>
-      <c r="C201" s="21" t="s">
-        <v>428</v>
+        <v>524</v>
+      </c>
+      <c r="C201" s="21">
+        <v>2700824260</v>
       </c>
       <c r="D201" s="19" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="14">
         <f t="shared" si="3"/>
         <v>201</v>
       </c>
       <c r="B202" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="C202" s="21">
-        <v>2700270679</v>
+        <v>525</v>
+      </c>
+      <c r="C202" s="21" t="s">
+        <v>429</v>
       </c>
       <c r="D202" s="19" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="14">
         <f t="shared" si="3"/>
         <v>202</v>
       </c>
       <c r="B203" s="20" t="s">
-        <v>525</v>
-      </c>
-      <c r="C203" s="21">
-        <v>2700824260</v>
+        <v>526</v>
+      </c>
+      <c r="C203" s="21" t="s">
+        <v>430</v>
       </c>
       <c r="D203" s="19" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="14">
         <f t="shared" si="3"/>
         <v>203</v>
       </c>
       <c r="B204" s="20" t="s">
-        <v>526</v>
-      </c>
-      <c r="C204" s="21" t="s">
-        <v>429</v>
+        <v>527</v>
+      </c>
+      <c r="C204" s="21">
+        <v>2700473809</v>
       </c>
       <c r="D204" s="19" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="14">
         <f t="shared" si="3"/>
         <v>204</v>
       </c>
       <c r="B205" s="20" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C205" s="21" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D205" s="19" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="14">
         <f t="shared" si="3"/>
         <v>205</v>
       </c>
       <c r="B206" s="20" t="s">
-        <v>528</v>
-      </c>
-      <c r="C206" s="21">
-        <v>2700473809</v>
+        <v>529</v>
+      </c>
+      <c r="C206" s="21" t="s">
+        <v>432</v>
       </c>
       <c r="D206" s="19" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="14">
         <f t="shared" si="3"/>
         <v>206</v>
       </c>
       <c r="B207" s="20" t="s">
-        <v>529</v>
-      </c>
-      <c r="C207" s="21" t="s">
-        <v>431</v>
+        <v>530</v>
+      </c>
+      <c r="C207" s="21">
+        <v>2500655142</v>
       </c>
       <c r="D207" s="19" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="14">
         <f t="shared" si="3"/>
         <v>207</v>
       </c>
       <c r="B208" s="20" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C208" s="21" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D208" s="19" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="14">
         <f t="shared" si="3"/>
         <v>208</v>
       </c>
       <c r="B209" s="20" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C209" s="21">
-        <v>2500655142</v>
+        <v>2500228415</v>
       </c>
       <c r="D209" s="19" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="14">
         <f t="shared" si="3"/>
         <v>209</v>
       </c>
       <c r="B210" s="20" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C210" s="21" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D210" s="19" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="14">
         <f t="shared" si="3"/>
         <v>210</v>
       </c>
       <c r="B211" s="20" t="s">
-        <v>533</v>
-      </c>
-      <c r="C211" s="21">
-        <v>2500228415</v>
+        <v>534</v>
+      </c>
+      <c r="C211" s="21" t="s">
+        <v>435</v>
       </c>
       <c r="D211" s="19" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="14">
         <f t="shared" si="3"/>
         <v>211</v>
       </c>
       <c r="B212" s="20" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C212" s="21" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D212" s="19" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="14">
         <f t="shared" si="3"/>
         <v>212</v>
       </c>
       <c r="B213" s="20" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C213" s="21" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D213" s="19" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="14">
         <f t="shared" si="3"/>
         <v>213</v>
       </c>
       <c r="B214" s="20" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C214" s="21" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="D214" s="19" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="14">
         <f t="shared" si="3"/>
         <v>214</v>
       </c>
       <c r="B215" s="20" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C215" s="21" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D215" s="19" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="14">
         <f t="shared" si="3"/>
         <v>215</v>
       </c>
       <c r="B216" s="20" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C216" s="21" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="D216" s="19" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="14">
         <f t="shared" si="3"/>
         <v>216</v>
       </c>
       <c r="B217" s="20" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C217" s="21" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D217" s="19" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="14">
         <f t="shared" si="3"/>
         <v>217</v>
       </c>
       <c r="B218" s="20" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C218" s="21" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D218" s="19" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="14">
         <f t="shared" si="3"/>
         <v>218</v>
       </c>
       <c r="B219" s="20" t="s">
-        <v>541</v>
-      </c>
-      <c r="C219" s="21" t="s">
-        <v>441</v>
+        <v>542</v>
+      </c>
+      <c r="C219" s="21">
+        <v>1500202535</v>
       </c>
       <c r="D219" s="19" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="14">
         <f t="shared" si="3"/>
         <v>219</v>
       </c>
       <c r="B220" s="20" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C220" s="21" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D220" s="19" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="14">
         <f t="shared" si="3"/>
         <v>220</v>
       </c>
       <c r="B221" s="20" t="s">
-        <v>543</v>
-      </c>
-      <c r="C221" s="21">
-        <v>1500202535</v>
+        <v>544</v>
+      </c>
+      <c r="C221" s="21" t="s">
+        <v>444</v>
       </c>
       <c r="D221" s="19" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="14">
         <f t="shared" si="3"/>
         <v>221</v>
       </c>
       <c r="B222" s="20" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C222" s="21" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D222" s="19" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="14">
         <f t="shared" si="3"/>
         <v>222</v>
       </c>
       <c r="B223" s="20" t="s">
-        <v>545</v>
-      </c>
-      <c r="C223" s="21" t="s">
-        <v>444</v>
+        <v>546</v>
+      </c>
+      <c r="C223" s="21">
+        <v>2500710509</v>
       </c>
       <c r="D223" s="19" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="14">
         <f t="shared" si="3"/>
         <v>223</v>
       </c>
       <c r="B224" s="20" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C224" s="21" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D224" s="19" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="14">
         <f t="shared" si="3"/>
         <v>224</v>
       </c>
       <c r="B225" s="20" t="s">
-        <v>547</v>
-      </c>
-      <c r="C225" s="21">
-        <v>2500710509</v>
+        <v>548</v>
+      </c>
+      <c r="C225" s="21" t="s">
+        <v>447</v>
       </c>
       <c r="D225" s="19" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="14">
         <f t="shared" si="3"/>
         <v>225</v>
       </c>
       <c r="B226" s="20" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C226" s="21" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="D226" s="19" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="14">
         <f t="shared" si="3"/>
         <v>226</v>
       </c>
       <c r="B227" s="20" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C227" s="21" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D227" s="19" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="14">
         <f t="shared" si="3"/>
         <v>227</v>
       </c>
       <c r="B228" s="20" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C228" s="21" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D228" s="19" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="14">
         <f t="shared" si="3"/>
         <v>228</v>
       </c>
       <c r="B229" s="20" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C229" s="21" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D229" s="19" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="14">
         <f t="shared" si="3"/>
         <v>229</v>
       </c>
       <c r="B230" s="20" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C230" s="21" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D230" s="19" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="14">
         <f t="shared" si="3"/>
         <v>230</v>
       </c>
       <c r="B231" s="20" t="s">
-        <v>553</v>
-      </c>
-      <c r="C231" s="21" t="s">
-        <v>451</v>
+        <v>554</v>
+      </c>
+      <c r="C231" s="21">
+        <v>1201619962</v>
       </c>
       <c r="D231" s="19" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="14">
         <f t="shared" si="3"/>
         <v>231</v>
       </c>
       <c r="B232" s="20" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C232" s="21" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D232" s="19" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" s="14">
         <f t="shared" si="3"/>
         <v>232</v>
       </c>
       <c r="B233" s="20" t="s">
-        <v>555</v>
-      </c>
-      <c r="C233" s="21">
-        <v>1201619962</v>
+        <v>556</v>
+      </c>
+      <c r="C233" s="21" t="s">
+        <v>454</v>
       </c>
       <c r="D233" s="19" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" s="14">
         <f t="shared" si="3"/>
         <v>233</v>
       </c>
       <c r="B234" s="20" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C234" s="21" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D234" s="19" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" s="14">
         <f t="shared" si="3"/>
         <v>234</v>
       </c>
       <c r="B235" s="20" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C235" s="21" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D235" s="19" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" s="14">
         <f t="shared" si="3"/>
         <v>235</v>
       </c>
       <c r="B236" s="20" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C236" s="21" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D236" s="19" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" s="14">
         <f t="shared" si="3"/>
         <v>236</v>
       </c>
       <c r="B237" s="20" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C237" s="21" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D237" s="19" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" s="14">
         <f t="shared" si="3"/>
         <v>237</v>
       </c>
       <c r="B238" s="20" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C238" s="21" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D238" s="19" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" s="14">
         <f t="shared" si="3"/>
         <v>238</v>
       </c>
       <c r="B239" s="20" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C239" s="21" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D239" s="19" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" s="14">
         <f t="shared" si="3"/>
         <v>239</v>
       </c>
       <c r="B240" s="20" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C240" s="21" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D240" s="19" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="14">
         <f t="shared" si="3"/>
         <v>240</v>
       </c>
       <c r="B241" s="20" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C241" s="21" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D241" s="19" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" s="14">
         <f t="shared" si="3"/>
         <v>241</v>
       </c>
       <c r="B242" s="20" t="s">
-        <v>564</v>
+        <v>677</v>
       </c>
       <c r="C242" s="21" t="s">
-        <v>461</v>
+        <v>678</v>
       </c>
       <c r="D242" s="19" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="14">
-        <f t="shared" si="3"/>
-        <v>242</v>
-      </c>
-      <c r="B243" s="20" t="s">
-        <v>565</v>
-      </c>
-      <c r="C243" s="21" t="s">
-        <v>462</v>
-      </c>
-      <c r="D243" s="19" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A244" s="14">
-        <f t="shared" si="3"/>
-        <v>243</v>
-      </c>
-      <c r="B244" s="20" t="s">
-        <v>680</v>
-      </c>
-      <c r="C244" s="21" t="s">
-        <v>681</v>
-      </c>
-      <c r="D244" s="19" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Cập nhật danh sách khách hàng
</commit_message>
<xml_diff>
--- a/DSKH.xlsx
+++ b/DSKH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB37E8A-B87A-4E78-93C0-25B3745B3A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7291B0B8-A0E5-4CD2-B10E-7B9B28507DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="831">
   <si>
     <t>STT</t>
   </si>
@@ -2493,6 +2493,42 @@
   </si>
   <si>
     <t>2700968985</t>
+  </si>
+  <si>
+    <t>VIỄN THÔNG NINH BÌNH  TẬP ĐOÀN BƯU CHÍNH VIỄN THÔNG VIỆT NAM</t>
+  </si>
+  <si>
+    <t>2700141673</t>
+  </si>
+  <si>
+    <t>KHTV.170</t>
+  </si>
+  <si>
+    <t>TỔNG CÔNG TY CỔ PHẦN BƯU CHÍNH VIETTEL</t>
+  </si>
+  <si>
+    <t>0104093672</t>
+  </si>
+  <si>
+    <t>KHTV.176</t>
+  </si>
+  <si>
+    <t>KHTV.175</t>
+  </si>
+  <si>
+    <t>0108461831</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH DỊCH VỤ DU LỊCH THỜI ĐẠI</t>
+  </si>
+  <si>
+    <t>KHTV.172</t>
+  </si>
+  <si>
+    <t>CÔNG TY CỔ PHẦN NAZ TECCON</t>
+  </si>
+  <si>
+    <t>0601304965</t>
   </si>
 </sst>
 </file>
@@ -2926,22 +2962,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E275"/>
+  <dimension ref="A1:E279"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D275" sqref="D275"/>
+    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
+      <selection activeCell="B280" sqref="B280"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2956,7 +2992,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -2971,7 +3007,7 @@
       </c>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <f>+A2+1</f>
         <v>2</v>
@@ -2987,7 +3023,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <f t="shared" ref="A4:A67" si="0">+A3+1</f>
         <v>3</v>
@@ -3003,7 +3039,7 @@
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3019,7 +3055,7 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3035,7 +3071,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3051,7 +3087,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3067,7 +3103,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3083,7 +3119,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3099,7 +3135,7 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3115,7 +3151,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3131,7 +3167,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3147,7 +3183,7 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3163,7 +3199,7 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3179,7 +3215,7 @@
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3195,7 +3231,7 @@
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3211,7 +3247,7 @@
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3227,7 +3263,7 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3243,7 +3279,7 @@
       </c>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3259,7 +3295,7 @@
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3275,7 +3311,7 @@
       </c>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3291,7 +3327,7 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3307,7 +3343,7 @@
       </c>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3323,7 +3359,7 @@
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3339,7 +3375,7 @@
       </c>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3355,7 +3391,7 @@
       </c>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3371,7 +3407,7 @@
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3387,7 +3423,7 @@
       </c>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3403,7 +3439,7 @@
       </c>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3419,7 +3455,7 @@
       </c>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3435,7 +3471,7 @@
       </c>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3451,7 +3487,7 @@
       </c>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3467,7 +3503,7 @@
       </c>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3483,7 +3519,7 @@
       </c>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3499,7 +3535,7 @@
       </c>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3515,7 +3551,7 @@
       </c>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3531,7 +3567,7 @@
       </c>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3547,7 +3583,7 @@
       </c>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3563,7 +3599,7 @@
       </c>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3579,7 +3615,7 @@
       </c>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3595,7 +3631,7 @@
       </c>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3611,7 +3647,7 @@
       </c>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3627,7 +3663,7 @@
       </c>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="8">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3643,7 +3679,7 @@
       </c>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3658,7 +3694,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3673,7 +3709,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3688,7 +3724,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="8">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3703,7 +3739,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -3718,7 +3754,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -3733,7 +3769,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -3748,7 +3784,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -3763,7 +3799,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -3778,7 +3814,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -3793,7 +3829,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="8">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -3808,7 +3844,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="8">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -3823,7 +3859,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -3838,7 +3874,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -3853,7 +3889,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -3868,7 +3904,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="8">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -3883,7 +3919,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="8">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -3898,7 +3934,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="8">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -3913,7 +3949,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="8">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -3928,7 +3964,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -3943,7 +3979,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="8">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -3958,7 +3994,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="8">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -3973,7 +4009,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="8">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -3988,7 +4024,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="8">
         <f t="shared" ref="A68:A131" si="1">+A67+1</f>
         <v>67</v>
@@ -4003,7 +4039,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="8">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -4018,7 +4054,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="8">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -4033,7 +4069,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="8">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -4048,7 +4084,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="8">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -4063,7 +4099,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="8">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -4078,7 +4114,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="8">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -4093,7 +4129,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="8">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -4108,7 +4144,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="8">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -4123,7 +4159,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="8">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -4138,7 +4174,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="8">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -4153,7 +4189,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="8">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -4168,7 +4204,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="8">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -4183,7 +4219,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="8">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -4198,7 +4234,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="8">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -4213,7 +4249,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="8">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -4228,7 +4264,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="8">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -4243,7 +4279,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="8">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -4258,7 +4294,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A86" s="8">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -4273,7 +4309,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="8">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -4288,7 +4324,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="8">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -4303,7 +4339,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="8">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -4318,7 +4354,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="8">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -4333,7 +4369,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="8">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -4348,7 +4384,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="8">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -4363,7 +4399,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="8">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -4378,7 +4414,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="8">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -4393,7 +4429,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="8">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -4408,7 +4444,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="8">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -4423,7 +4459,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="8">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -4438,7 +4474,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="8">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -4451,7 +4487,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="8">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -4464,7 +4500,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="8">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -4477,7 +4513,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="8">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4492,7 +4528,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="8">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -4507,7 +4543,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="8">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -4520,7 +4556,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="8">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -4533,7 +4569,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="8">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -4548,7 +4584,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="8">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -4563,7 +4599,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="8">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -4578,7 +4614,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="8">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -4593,7 +4629,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="8">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -4608,7 +4644,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="8">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -4623,7 +4659,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="8">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -4638,7 +4674,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="8">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -4653,7 +4689,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="8">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -4668,7 +4704,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="8">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -4683,7 +4719,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="8">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -4698,7 +4734,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="8">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -4713,7 +4749,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="8">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -4728,7 +4764,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="8">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -4743,7 +4779,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="8">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -4758,7 +4794,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="8">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -4773,7 +4809,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="8">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -4788,7 +4824,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="8">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -4803,7 +4839,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="8">
         <f t="shared" si="1"/>
         <v>122</v>
@@ -4818,7 +4854,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="8">
         <f t="shared" si="1"/>
         <v>123</v>
@@ -4833,7 +4869,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="8">
         <f t="shared" si="1"/>
         <v>124</v>
@@ -4848,7 +4884,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="8">
         <f t="shared" si="1"/>
         <v>125</v>
@@ -4863,7 +4899,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="8">
         <f t="shared" si="1"/>
         <v>126</v>
@@ -4878,7 +4914,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="8">
         <f t="shared" si="1"/>
         <v>127</v>
@@ -4893,7 +4929,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="8">
         <f t="shared" si="1"/>
         <v>128</v>
@@ -4908,7 +4944,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="8">
         <f t="shared" si="1"/>
         <v>129</v>
@@ -4923,7 +4959,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="8">
         <f t="shared" si="1"/>
         <v>130</v>
@@ -4938,7 +4974,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="8">
         <f t="shared" ref="A132:A195" si="2">+A131+1</f>
         <v>131</v>
@@ -4953,7 +4989,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="8">
         <f t="shared" si="2"/>
         <v>132</v>
@@ -4968,7 +5004,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="8">
         <f t="shared" si="2"/>
         <v>133</v>
@@ -4983,7 +5019,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="8">
         <f t="shared" si="2"/>
         <v>134</v>
@@ -4998,7 +5034,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="8">
         <f t="shared" si="2"/>
         <v>135</v>
@@ -5013,7 +5049,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A137" s="8">
         <f t="shared" si="2"/>
         <v>136</v>
@@ -5028,7 +5064,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="8">
         <f t="shared" si="2"/>
         <v>137</v>
@@ -5043,7 +5079,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="8">
         <f t="shared" si="2"/>
         <v>138</v>
@@ -5058,7 +5094,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="8">
         <f t="shared" si="2"/>
         <v>139</v>
@@ -5073,7 +5109,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="8">
         <f t="shared" si="2"/>
         <v>140</v>
@@ -5088,7 +5124,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="8">
         <f t="shared" si="2"/>
         <v>141</v>
@@ -5103,7 +5139,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="8">
         <f t="shared" si="2"/>
         <v>142</v>
@@ -5118,7 +5154,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="8">
         <f t="shared" si="2"/>
         <v>143</v>
@@ -5133,7 +5169,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="8">
         <f t="shared" si="2"/>
         <v>144</v>
@@ -5148,7 +5184,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="8">
         <f t="shared" si="2"/>
         <v>145</v>
@@ -5163,7 +5199,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="8">
         <f t="shared" si="2"/>
         <v>146</v>
@@ -5176,7 +5212,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="8">
         <f t="shared" si="2"/>
         <v>147</v>
@@ -5191,7 +5227,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="8">
         <f t="shared" si="2"/>
         <v>148</v>
@@ -5206,7 +5242,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="8">
         <f t="shared" si="2"/>
         <v>149</v>
@@ -5221,7 +5257,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="8">
         <f t="shared" si="2"/>
         <v>150</v>
@@ -5236,7 +5272,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="8">
         <f t="shared" si="2"/>
         <v>151</v>
@@ -5251,7 +5287,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="8">
         <f t="shared" si="2"/>
         <v>152</v>
@@ -5266,7 +5302,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="8">
         <f t="shared" si="2"/>
         <v>153</v>
@@ -5281,7 +5317,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="8">
         <f t="shared" si="2"/>
         <v>154</v>
@@ -5296,7 +5332,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="8">
         <f t="shared" si="2"/>
         <v>155</v>
@@ -5311,7 +5347,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="8">
         <f t="shared" si="2"/>
         <v>156</v>
@@ -5326,7 +5362,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="8">
         <f t="shared" si="2"/>
         <v>157</v>
@@ -5341,7 +5377,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="8">
         <f t="shared" si="2"/>
         <v>158</v>
@@ -5356,7 +5392,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="8">
         <f t="shared" si="2"/>
         <v>159</v>
@@ -5371,7 +5407,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="8">
         <f t="shared" si="2"/>
         <v>160</v>
@@ -5386,7 +5422,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="8">
         <f t="shared" si="2"/>
         <v>161</v>
@@ -5401,7 +5437,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="8">
         <f t="shared" si="2"/>
         <v>162</v>
@@ -5416,7 +5452,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="8">
         <f t="shared" si="2"/>
         <v>163</v>
@@ -5431,7 +5467,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="8">
         <f t="shared" si="2"/>
         <v>164</v>
@@ -5446,7 +5482,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="8">
         <f t="shared" si="2"/>
         <v>165</v>
@@ -5461,7 +5497,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="8">
         <f t="shared" si="2"/>
         <v>166</v>
@@ -5476,7 +5512,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="8">
         <f t="shared" si="2"/>
         <v>167</v>
@@ -5491,7 +5527,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="8">
         <f t="shared" si="2"/>
         <v>168</v>
@@ -5506,7 +5542,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="8">
         <f t="shared" si="2"/>
         <v>169</v>
@@ -5521,7 +5557,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="8">
         <f t="shared" si="2"/>
         <v>170</v>
@@ -5536,7 +5572,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="8">
         <f t="shared" si="2"/>
         <v>171</v>
@@ -5551,7 +5587,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="8">
         <f t="shared" si="2"/>
         <v>172</v>
@@ -5566,7 +5602,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="8">
         <f t="shared" si="2"/>
         <v>173</v>
@@ -5581,7 +5617,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="8">
         <f t="shared" si="2"/>
         <v>174</v>
@@ -5596,7 +5632,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="8">
         <f t="shared" si="2"/>
         <v>175</v>
@@ -5611,7 +5647,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="8">
         <f t="shared" si="2"/>
         <v>176</v>
@@ -5626,7 +5662,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="8">
         <f t="shared" si="2"/>
         <v>177</v>
@@ -5641,7 +5677,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="8">
         <f t="shared" si="2"/>
         <v>178</v>
@@ -5656,7 +5692,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="8">
         <f t="shared" si="2"/>
         <v>179</v>
@@ -5671,7 +5707,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A181" s="8">
         <f t="shared" si="2"/>
         <v>180</v>
@@ -5686,7 +5722,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="8">
         <f t="shared" si="2"/>
         <v>181</v>
@@ -5701,7 +5737,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="8">
         <f t="shared" si="2"/>
         <v>182</v>
@@ -5716,7 +5752,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="8">
         <f t="shared" si="2"/>
         <v>183</v>
@@ -5731,7 +5767,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="8">
         <f t="shared" si="2"/>
         <v>184</v>
@@ -5746,7 +5782,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="8">
         <f t="shared" si="2"/>
         <v>185</v>
@@ -5761,7 +5797,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="8">
         <f t="shared" si="2"/>
         <v>186</v>
@@ -5776,7 +5812,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="8">
         <f t="shared" si="2"/>
         <v>187</v>
@@ -5791,7 +5827,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="8">
         <f t="shared" si="2"/>
         <v>188</v>
@@ -5806,7 +5842,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="8">
         <f t="shared" si="2"/>
         <v>189</v>
@@ -5821,7 +5857,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="8">
         <f t="shared" si="2"/>
         <v>190</v>
@@ -5836,7 +5872,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="8">
         <f t="shared" si="2"/>
         <v>191</v>
@@ -5851,7 +5887,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="8">
         <f t="shared" si="2"/>
         <v>192</v>
@@ -5866,7 +5902,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="8">
         <f t="shared" si="2"/>
         <v>193</v>
@@ -5881,7 +5917,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="8">
         <f t="shared" si="2"/>
         <v>194</v>
@@ -5896,7 +5932,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="8">
         <f t="shared" ref="A196:A259" si="3">+A195+1</f>
         <v>195</v>
@@ -5911,7 +5947,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="8">
         <f t="shared" si="3"/>
         <v>196</v>
@@ -5926,7 +5962,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="8">
         <f t="shared" si="3"/>
         <v>197</v>
@@ -5941,7 +5977,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="8">
         <f t="shared" si="3"/>
         <v>198</v>
@@ -5956,7 +5992,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="8">
         <f t="shared" si="3"/>
         <v>199</v>
@@ -5971,7 +6007,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="8">
         <f t="shared" si="3"/>
         <v>200</v>
@@ -5986,7 +6022,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="8">
         <f t="shared" si="3"/>
         <v>201</v>
@@ -6001,7 +6037,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="8">
         <f t="shared" si="3"/>
         <v>202</v>
@@ -6016,7 +6052,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="8">
         <f t="shared" si="3"/>
         <v>203</v>
@@ -6031,7 +6067,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="8">
         <f t="shared" si="3"/>
         <v>204</v>
@@ -6046,7 +6082,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="8">
         <f t="shared" si="3"/>
         <v>205</v>
@@ -6061,7 +6097,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="8">
         <f t="shared" si="3"/>
         <v>206</v>
@@ -6076,7 +6112,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="8">
         <f t="shared" si="3"/>
         <v>207</v>
@@ -6091,7 +6127,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="8">
         <f t="shared" si="3"/>
         <v>208</v>
@@ -6106,7 +6142,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="8">
         <f t="shared" si="3"/>
         <v>209</v>
@@ -6121,7 +6157,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="8">
         <f t="shared" si="3"/>
         <v>210</v>
@@ -6136,7 +6172,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="8">
         <f t="shared" si="3"/>
         <v>211</v>
@@ -6151,7 +6187,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="8">
         <f t="shared" si="3"/>
         <v>212</v>
@@ -6166,7 +6202,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="8">
         <f t="shared" si="3"/>
         <v>213</v>
@@ -6181,7 +6217,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="8">
         <f t="shared" si="3"/>
         <v>214</v>
@@ -6196,7 +6232,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="8">
         <f t="shared" si="3"/>
         <v>215</v>
@@ -6211,7 +6247,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="8">
         <f t="shared" si="3"/>
         <v>216</v>
@@ -6226,7 +6262,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="8">
         <f t="shared" si="3"/>
         <v>217</v>
@@ -6241,7 +6277,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="8">
         <f t="shared" si="3"/>
         <v>218</v>
@@ -6256,7 +6292,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="8">
         <f t="shared" si="3"/>
         <v>219</v>
@@ -6271,7 +6307,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="8">
         <f t="shared" si="3"/>
         <v>220</v>
@@ -6286,7 +6322,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="8">
         <f t="shared" si="3"/>
         <v>221</v>
@@ -6301,7 +6337,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="8">
         <f t="shared" si="3"/>
         <v>222</v>
@@ -6316,7 +6352,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="8">
         <f t="shared" si="3"/>
         <v>223</v>
@@ -6331,7 +6367,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="8">
         <f t="shared" si="3"/>
         <v>224</v>
@@ -6346,7 +6382,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="8">
         <f t="shared" si="3"/>
         <v>225</v>
@@ -6361,7 +6397,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="8">
         <f t="shared" si="3"/>
         <v>226</v>
@@ -6376,7 +6412,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="8">
         <f t="shared" si="3"/>
         <v>227</v>
@@ -6391,7 +6427,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="8">
         <f t="shared" si="3"/>
         <v>228</v>
@@ -6406,7 +6442,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="8">
         <f t="shared" si="3"/>
         <v>229</v>
@@ -6421,7 +6457,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="8">
         <f t="shared" si="3"/>
         <v>230</v>
@@ -6436,7 +6472,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="8">
         <f t="shared" si="3"/>
         <v>231</v>
@@ -6451,7 +6487,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" s="8">
         <f t="shared" si="3"/>
         <v>232</v>
@@ -6466,7 +6502,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" s="8">
         <f t="shared" si="3"/>
         <v>233</v>
@@ -6481,7 +6517,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" s="8">
         <f t="shared" si="3"/>
         <v>234</v>
@@ -6496,7 +6532,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" s="8">
         <f t="shared" si="3"/>
         <v>235</v>
@@ -6511,7 +6547,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" s="8">
         <f t="shared" si="3"/>
         <v>236</v>
@@ -6526,7 +6562,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" s="8">
         <f t="shared" si="3"/>
         <v>237</v>
@@ -6541,7 +6577,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" s="8">
         <f t="shared" si="3"/>
         <v>238</v>
@@ -6556,7 +6592,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" s="8">
         <f t="shared" si="3"/>
         <v>239</v>
@@ -6571,7 +6607,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="8">
         <f t="shared" si="3"/>
         <v>240</v>
@@ -6586,7 +6622,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" s="8">
         <f t="shared" si="3"/>
         <v>241</v>
@@ -6601,7 +6637,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" s="8">
         <f t="shared" si="3"/>
         <v>242</v>
@@ -6616,7 +6652,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" s="8">
         <f t="shared" si="3"/>
         <v>243</v>
@@ -6631,7 +6667,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" s="8">
         <f t="shared" si="3"/>
         <v>244</v>
@@ -6646,7 +6682,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" s="8">
         <f t="shared" si="3"/>
         <v>245</v>
@@ -6661,7 +6697,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="8">
         <f t="shared" si="3"/>
         <v>246</v>
@@ -6676,7 +6712,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" s="8">
         <f t="shared" si="3"/>
         <v>247</v>
@@ -6691,7 +6727,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" s="8">
         <f t="shared" si="3"/>
         <v>248</v>
@@ -6706,7 +6742,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" s="8">
         <f t="shared" si="3"/>
         <v>249</v>
@@ -6721,7 +6757,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" s="8">
         <f t="shared" si="3"/>
         <v>250</v>
@@ -6736,7 +6772,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252" s="8">
         <f t="shared" si="3"/>
         <v>251</v>
@@ -6751,7 +6787,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" s="8">
         <f t="shared" si="3"/>
         <v>252</v>
@@ -6766,7 +6802,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" s="8">
         <f t="shared" si="3"/>
         <v>253</v>
@@ -6781,7 +6817,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255" s="8">
         <f t="shared" si="3"/>
         <v>254</v>
@@ -6796,7 +6832,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" s="8">
         <f t="shared" si="3"/>
         <v>255</v>
@@ -6811,7 +6847,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A257" s="8">
         <f t="shared" si="3"/>
         <v>256</v>
@@ -6826,7 +6862,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258" s="8">
         <f t="shared" si="3"/>
         <v>257</v>
@@ -6841,7 +6877,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259" s="8">
         <f t="shared" si="3"/>
         <v>258</v>
@@ -6856,9 +6892,9 @@
         <v>730</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260" s="8">
-        <f t="shared" ref="A260:A275" si="4">+A259+1</f>
+        <f t="shared" ref="A260:A279" si="4">+A259+1</f>
         <v>259</v>
       </c>
       <c r="B260" s="9" t="s">
@@ -6871,7 +6907,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261" s="8">
         <f t="shared" si="4"/>
         <v>260</v>
@@ -6886,7 +6922,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262" s="8">
         <f t="shared" si="4"/>
         <v>261</v>
@@ -6901,7 +6937,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263" s="8">
         <f t="shared" si="4"/>
         <v>262</v>
@@ -6916,7 +6952,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264" s="8">
         <f t="shared" si="4"/>
         <v>263</v>
@@ -6931,7 +6967,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265" s="8">
         <f t="shared" si="4"/>
         <v>264</v>
@@ -6946,7 +6982,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266" s="8">
         <f t="shared" si="4"/>
         <v>265</v>
@@ -6961,7 +6997,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267" s="8">
         <f t="shared" si="4"/>
         <v>266</v>
@@ -6974,7 +7010,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268" s="8">
         <f t="shared" si="4"/>
         <v>267</v>
@@ -6989,7 +7025,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269" s="8">
         <f t="shared" si="4"/>
         <v>268</v>
@@ -7004,7 +7040,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270" s="8">
         <f t="shared" si="4"/>
         <v>269</v>
@@ -7019,7 +7055,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271" s="8">
         <f t="shared" si="4"/>
         <v>270</v>
@@ -7034,7 +7070,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272" s="8">
         <f t="shared" si="4"/>
         <v>271</v>
@@ -7049,7 +7085,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273" s="8">
         <f t="shared" si="4"/>
         <v>272</v>
@@ -7064,7 +7100,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274" s="8">
         <f t="shared" si="4"/>
         <v>273</v>
@@ -7079,7 +7115,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275" s="8">
         <f t="shared" si="4"/>
         <v>274</v>
@@ -7094,11 +7130,71 @@
         <v>745</v>
       </c>
     </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A276" s="8">
+        <f t="shared" si="4"/>
+        <v>275</v>
+      </c>
+      <c r="B276" s="9" t="s">
+        <v>819</v>
+      </c>
+      <c r="C276" s="9" t="s">
+        <v>820</v>
+      </c>
+      <c r="D276" s="9" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A277" s="8">
+        <f t="shared" si="4"/>
+        <v>276</v>
+      </c>
+      <c r="B277" s="9" t="s">
+        <v>822</v>
+      </c>
+      <c r="C277" s="9" t="s">
+        <v>823</v>
+      </c>
+      <c r="D277" s="9" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A278" s="8">
+        <f t="shared" si="4"/>
+        <v>277</v>
+      </c>
+      <c r="B278" s="9" t="s">
+        <v>827</v>
+      </c>
+      <c r="C278" s="9" t="s">
+        <v>826</v>
+      </c>
+      <c r="D278" s="9" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A279" s="8">
+        <f t="shared" si="4"/>
+        <v>278</v>
+      </c>
+      <c r="B279" s="9" t="s">
+        <v>829</v>
+      </c>
+      <c r="C279" s="9" t="s">
+        <v>830</v>
+      </c>
+      <c r="D279" s="9" t="s">
+        <v>828</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C1:C275 C280:C1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D276:D1048576 D1">
+  <conditionalFormatting sqref="D280:D1048576 D1">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cập nhật DSKH Lộc Hạ
</commit_message>
<xml_diff>
--- a/DSKH.xlsx
+++ b/DSKH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Works 2\IT\GITHUB\UpSSE_render\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3BDE4D-D030-4F8D-8048-985EDABAE67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5912F65-0B7E-4119-B429-B0E509623B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="840">
   <si>
     <t>STT</t>
   </si>
@@ -2529,6 +2529,33 @@
   </si>
   <si>
     <t>0601304965</t>
+  </si>
+  <si>
+    <t>NGUYỄN MINH THẮNG</t>
+  </si>
+  <si>
+    <t>KHTV.165</t>
+  </si>
+  <si>
+    <t>035090004075</t>
+  </si>
+  <si>
+    <t>Công ty TNHH Bách Đại Phát</t>
+  </si>
+  <si>
+    <t>0601043953</t>
+  </si>
+  <si>
+    <t>BL060010</t>
+  </si>
+  <si>
+    <t>Công ty Cổ phần tư vấn và xây dựng Hà Ninh</t>
+  </si>
+  <si>
+    <t>0600945194</t>
+  </si>
+  <si>
+    <t>BL004004</t>
   </si>
 </sst>
 </file>
@@ -2538,7 +2565,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2591,6 +2618,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2641,7 +2674,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2686,6 +2719,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2962,10 +2999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E279"/>
+  <dimension ref="A1:E282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
-      <selection activeCell="B273" sqref="B273"/>
+    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
+      <selection activeCell="B282" sqref="B282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -6894,7 +6931,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260" s="8">
-        <f t="shared" ref="A260:A279" si="4">+A259+1</f>
+        <f t="shared" ref="A260:A282" si="4">+A259+1</f>
         <v>259</v>
       </c>
       <c r="B260" s="9" t="s">
@@ -7190,14 +7227,60 @@
         <v>828</v>
       </c>
     </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A280" s="8">
+        <f t="shared" si="4"/>
+        <v>279</v>
+      </c>
+      <c r="B280" s="9" t="s">
+        <v>831</v>
+      </c>
+      <c r="C280" s="20" t="s">
+        <v>833</v>
+      </c>
+      <c r="D280" s="9" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A281" s="8">
+        <f t="shared" si="4"/>
+        <v>280</v>
+      </c>
+      <c r="B281" s="21" t="s">
+        <v>834</v>
+      </c>
+      <c r="C281" s="20" t="s">
+        <v>835</v>
+      </c>
+      <c r="D281" s="21" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A282" s="8">
+        <f t="shared" si="4"/>
+        <v>281</v>
+      </c>
+      <c r="B282" s="21" t="s">
+        <v>837</v>
+      </c>
+      <c r="C282" s="20" t="s">
+        <v>838</v>
+      </c>
+      <c r="D282" s="21" t="s">
+        <v>839</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C275 C280:C1048576">
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="C1:C275 C283:C1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D280:D1048576 D1">
+  <conditionalFormatting sqref="D281:D1048576 D1">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>